<commit_message>
Hoan Thien Ung Dung
</commit_message>
<xml_diff>
--- a/BaoCaoThongKeNam2023.xlsx
+++ b/BaoCaoThongKeNam2023.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="17">
   <si>
     <t/>
   </si>
@@ -32,19 +32,37 @@
     <t>Tổng tiền</t>
   </si>
   <si>
-    <t>Giày Méo Méo Méo</t>
+    <t>Adidas Samba</t>
+  </si>
+  <si>
+    <t>Air Runner</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Nike Air Force 1</t>
+  </si>
+  <si>
+    <t>Nike Air Force Limited</t>
+  </si>
+  <si>
+    <t>Nike Runner 3</t>
+  </si>
+  <si>
+    <t>San Pham Mau test</t>
+  </si>
+  <si>
+    <t>Vans VanGoal</t>
+  </si>
+  <si>
+    <t>Vans Vault</t>
+  </si>
+  <si>
+    <t>Yeeze</t>
   </si>
   <si>
     <t>Nike Runner</t>
-  </si>
-  <si>
-    <t>Nike Runner 3</t>
-  </si>
-  <si>
-    <t>GIày Của Long</t>
-  </si>
-  <si>
-    <t>Nike Air Force 1</t>
   </si>
 </sst>
 </file>
@@ -89,7 +107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:D14"/>
+  <dimension ref="A2:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -116,142 +134,436 @@
     </row>
     <row r="5">
       <c r="A5" t="n" s="0">
-        <v>3.0</v>
+        <v>12.0</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>6</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>40.0</v>
+        <v>1.0</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>90.0</v>
+        <v>4400000.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n" s="0">
-        <v>3.0</v>
+        <v>12.0</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>7</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>74.0</v>
+        <v>1.0</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>90.0</v>
+        <v>6.0676663E7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n" s="0">
-        <v>3.0</v>
+        <v>12.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="n" s="0">
-        <v>60.0</v>
+        <v>2.0</v>
       </c>
       <c r="D7" t="n" s="0">
-        <v>90.0</v>
+        <v>2.05E7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n" s="0">
-        <v>2.0</v>
+        <v>12.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" t="n" s="0">
-        <v>39.0</v>
+        <v>3.0</v>
       </c>
       <c r="D8" t="n" s="0">
-        <v>140.0</v>
+        <v>1.434333E7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n" s="0">
-        <v>2.0</v>
+        <v>12.0</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>40.0</v>
+        <v>5.0</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>70.0</v>
+        <v>1.15E7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n" s="0">
-        <v>2.0</v>
+        <v>12.0</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" t="n" s="0">
-        <v>100.0</v>
+        <v>1.0</v>
       </c>
       <c r="D10" t="n" s="0">
-        <v>70.0</v>
+        <v>4.8646661E7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C11" t="n" s="0">
         <v>2.0</v>
       </c>
-      <c r="B11" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C11" t="n" s="0">
-        <v>74.0</v>
-      </c>
       <c r="D11" t="n" s="0">
-        <v>70.0</v>
+        <v>9813330.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n" s="0">
-        <v>1.0</v>
+        <v>12.0</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" t="n" s="0">
-        <v>39.0</v>
+        <v>4.0</v>
       </c>
       <c r="D12" t="n" s="0">
-        <v>480.0</v>
+        <v>5600000.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n" s="0">
-        <v>1.0</v>
+        <v>12.0</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="n" s="0">
-        <v>100.0</v>
+        <v>1.0</v>
       </c>
       <c r="D13" t="n" s="0">
-        <v>80.0</v>
+        <v>3.266E7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n" s="0">
-        <v>1.0</v>
+        <v>12.0</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" t="n" s="0">
-        <v>60.0</v>
+        <v>4.0</v>
       </c>
       <c r="D14" t="n" s="0">
-        <v>80.0</v>
+        <v>1.2E8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C15" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D15" t="n" s="0">
+        <v>5.021E7</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C16" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="D16" t="n" s="0">
+        <v>1.002E7</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C17" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D17" t="n" s="0">
+        <v>4.54E7</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C18" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D18" t="n" s="0">
+        <v>7150000.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C19" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D19" t="n" s="0">
+        <v>3240000.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C20" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="D20" t="n" s="0">
+        <v>3240000.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C21" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="D21" t="n" s="0">
+        <v>1.002E7</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C22" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D22" t="n" s="0">
+        <v>1.922E7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C23" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="D23" t="n" s="0">
+        <v>1.214E7</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C24" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D24" t="n" s="0">
+        <v>5.6706663E7</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C25" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="D25" t="n" s="0">
+        <v>80000.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C26" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="D26" t="n" s="0">
+        <v>2.092E7</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C27" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="D27" t="n" s="0">
+        <v>1.214E7</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C28" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="D28" t="n" s="0">
+        <v>3.1373333E7</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C29" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D29" t="n" s="0">
+        <v>200000.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C30" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D30" t="n" s="0">
+        <v>2200000.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C31" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D31" t="n" s="0">
+        <v>240000.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C32" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="D32" t="n" s="0">
+        <v>6600000.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C33" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D33" t="n" s="0">
+        <v>2400000.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C34" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D34" t="n" s="0">
+        <v>200000.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C35" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D35" t="n" s="0">
+        <v>200000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>